<commit_message>
added AYTO VIP S2 Episode 11 results
</commit_message>
<xml_diff>
--- a/results/AYTO VIP S2/results.xlsx
+++ b/results/AYTO VIP S2/results.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Episode 08" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Episode 09" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Episode 10" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Episode 11" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1323,6 +1324,482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amadu</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Luca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lukas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maurice</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pharrell</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B2" s="56" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="E2" s="40" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="22" t="n">
+        <v>0.1733333333333333</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="J2" s="57" t="n">
+        <v>0.3633333333333333</v>
+      </c>
+      <c r="K2" s="58" t="n">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cecilia</t>
+        </is>
+      </c>
+      <c r="B3" s="59" t="n">
+        <v>0.6866666666666666</v>
+      </c>
+      <c r="C3" s="56" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="D3" s="40" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="18" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="40" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="56" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="J3" s="47" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="K3" s="46" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L3" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Celina</t>
+        </is>
+      </c>
+      <c r="B4" s="18" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="D4" s="60" t="n">
+        <v>0.2366666666666667</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>0.06333333333333334</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H4" s="36" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="I4" s="46" t="n">
+        <v>0.09333333333333334</v>
+      </c>
+      <c r="J4" s="41" t="n">
+        <v>0.08666666666666667</v>
+      </c>
+      <c r="K4" s="61" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Franziska</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="D5" s="24" t="n">
+        <v>0.1033333333333333</v>
+      </c>
+      <c r="E5" s="62" t="n">
+        <v>0.1233333333333333</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="27" t="n">
+        <v>0.1133333333333333</v>
+      </c>
+      <c r="H5" s="43" t="n">
+        <v>0.01666666666666667</v>
+      </c>
+      <c r="I5" s="53" t="n">
+        <v>0.2566666666666667</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="K5" s="63" t="n">
+        <v>0.1533333333333333</v>
+      </c>
+      <c r="L5" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+      <c r="B6" s="47" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="C6" s="53" t="n">
+        <v>0.2566666666666667</v>
+      </c>
+      <c r="D6" s="24" t="n">
+        <v>0.1033333333333333</v>
+      </c>
+      <c r="E6" s="38" t="n">
+        <v>0.09666666666666666</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="46" t="n">
+        <v>0.09333333333333334</v>
+      </c>
+      <c r="H6" s="54" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="13" t="n">
+        <v>0.1066666666666667</v>
+      </c>
+      <c r="J6" s="48" t="n">
+        <v>0.1466666666666667</v>
+      </c>
+      <c r="K6" s="61" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="L6" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="B7" s="15" t="n">
+        <v>0.05666666666666666</v>
+      </c>
+      <c r="C7" s="20" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D7" s="46" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E7" s="29" t="n">
+        <v>0.2633333333333333</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="22" t="n">
+        <v>0.1733333333333333</v>
+      </c>
+      <c r="H7" s="64" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I7" s="46" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="J7" s="38" t="n">
+        <v>0.09666666666666666</v>
+      </c>
+      <c r="K7" s="52" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Karina</t>
+        </is>
+      </c>
+      <c r="B8" s="16" t="n">
+        <v>0.05333333333333334</v>
+      </c>
+      <c r="C8" s="65" t="n">
+        <v>0.3133333333333334</v>
+      </c>
+      <c r="D8" s="66" t="n">
+        <v>0.1966666666666667</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="58" t="n">
+        <v>0.1366666666666667</v>
+      </c>
+      <c r="H8" s="36" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Luisa</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Ricarda</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="36" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="D10" s="36" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="E10" s="64" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="64" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H10" s="68" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="I10" s="36" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="47" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="B11" s="34" t="n">
+        <v>0.04666666666666667</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>0.07333333333333333</v>
+      </c>
+      <c r="D11" s="24" t="n">
+        <v>0.1033333333333333</v>
+      </c>
+      <c r="E11" s="51" t="n">
+        <v>0.2533333333333334</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="36" t="n">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="I11" s="69" t="n">
+        <v>0.2466666666666667</v>
+      </c>
+      <c r="J11" s="27" t="n">
+        <v>0.1133333333333333</v>
+      </c>
+      <c r="K11" s="70" t="n">
+        <v>0.1566666666666667</v>
+      </c>
+      <c r="L11" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added AYTO VIP S2 Episode 12 results
</commit_message>
<xml_diff>
--- a/results/AYTO VIP S2/results.xlsx
+++ b/results/AYTO VIP S2/results.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Episode 09" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Episode 10" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Episode 11" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Episode 12" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44,7 +45,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="71">
+  <fills count="84">
     <fill>
       <patternFill/>
     </fill>
@@ -394,6 +395,71 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0028D7FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CD32FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0003FCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003DC2FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0009F6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002BD4FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004CB3FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003AC5FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EB14FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00629DFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002FD0FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002DD2FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0021DEFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -415,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -489,6 +555,19 @@
     <xf numFmtId="0" fontId="3" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="70" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="75" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="80" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="71" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="72" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="74" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="81" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="73" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="82" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="83" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="76" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="78" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="79" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="77" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1800,6 +1879,482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amadu</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Luca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lukas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maurice</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pharrell</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B2" s="18" t="n">
+        <v>0.02876106194690265</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>0.06305309734513274</v>
+      </c>
+      <c r="D2" s="38" t="n">
+        <v>0.09734513274336283</v>
+      </c>
+      <c r="E2" s="71" t="n">
+        <v>0.03650442477876106</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="35" t="n">
+        <v>0.163716814159292</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11" t="n">
+        <v>0.06305309734513274</v>
+      </c>
+      <c r="J2" s="72" t="n">
+        <v>0.3838495575221239</v>
+      </c>
+      <c r="K2" s="35" t="n">
+        <v>0.163716814159292</v>
+      </c>
+      <c r="L2" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cecilia</t>
+        </is>
+      </c>
+      <c r="B3" s="73" t="n">
+        <v>0.8030973451327433</v>
+      </c>
+      <c r="C3" s="54" t="n">
+        <v>0.02212389380530973</v>
+      </c>
+      <c r="D3" s="74" t="n">
+        <v>0.01548672566371681</v>
+      </c>
+      <c r="E3" s="54" t="n">
+        <v>0.02101769911504425</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="56" t="n">
+        <v>0.03429203539823009</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="34" t="n">
+        <v>0.04535398230088496</v>
+      </c>
+      <c r="J3" s="74" t="n">
+        <v>0.01216814159292035</v>
+      </c>
+      <c r="K3" s="34" t="n">
+        <v>0.04646017699115045</v>
+      </c>
+      <c r="L3" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Celina</t>
+        </is>
+      </c>
+      <c r="B4" s="74" t="n">
+        <v>0.01216814159292035</v>
+      </c>
+      <c r="C4" s="46" t="n">
+        <v>0.09292035398230089</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>0.3252212389380531</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0.08296460176991151</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="35" t="n">
+        <v>0.1615044247787611</v>
+      </c>
+      <c r="H4" s="75" t="n">
+        <v>0.002212389380530973</v>
+      </c>
+      <c r="I4" s="38" t="n">
+        <v>0.09402654867256637</v>
+      </c>
+      <c r="J4" s="24" t="n">
+        <v>0.1028761061946903</v>
+      </c>
+      <c r="K4" s="33" t="n">
+        <v>0.1261061946902655</v>
+      </c>
+      <c r="L4" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Franziska</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>0.06858407079646017</v>
+      </c>
+      <c r="C5" s="62" t="n">
+        <v>0.1216814159292035</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.09955752212389381</v>
+      </c>
+      <c r="E5" s="14" t="n">
+        <v>0.120575221238938</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33" t="n">
+        <v>0.127212389380531</v>
+      </c>
+      <c r="H5" s="64" t="n">
+        <v>0.01106194690265487</v>
+      </c>
+      <c r="I5" s="42" t="n">
+        <v>0.1935840707964602</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>0.07190265486725664</v>
+      </c>
+      <c r="K5" s="76" t="n">
+        <v>0.1858407079646018</v>
+      </c>
+      <c r="L5" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+      <c r="B6" s="74" t="n">
+        <v>0.01438053097345133</v>
+      </c>
+      <c r="C6" s="77" t="n">
+        <v>0.2400442477876106</v>
+      </c>
+      <c r="D6" s="46" t="n">
+        <v>0.09292035398230089</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0.1106194690265487</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="41" t="n">
+        <v>0.08738938053097345</v>
+      </c>
+      <c r="H6" s="74" t="n">
+        <v>0.01327433628318584</v>
+      </c>
+      <c r="I6" s="63" t="n">
+        <v>0.1559734513274336</v>
+      </c>
+      <c r="J6" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+      <c r="K6" s="78" t="n">
+        <v>0.1769911504424779</v>
+      </c>
+      <c r="L6" s="79" t="n">
+        <v>0.1327433628318584</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="B7" s="34" t="n">
+        <v>0.04314159292035398</v>
+      </c>
+      <c r="C7" s="27" t="n">
+        <v>0.1139380530973451</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.07743362831858407</v>
+      </c>
+      <c r="E7" s="80" t="n">
+        <v>0.168141592920354</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="81" t="n">
+        <v>0.2267699115044248</v>
+      </c>
+      <c r="H7" s="43" t="n">
+        <v>0.01769911504424779</v>
+      </c>
+      <c r="I7" s="46" t="n">
+        <v>0.09292035398230089</v>
+      </c>
+      <c r="J7" s="24" t="n">
+        <v>0.1050884955752212</v>
+      </c>
+      <c r="K7" s="63" t="n">
+        <v>0.1548672566371681</v>
+      </c>
+      <c r="L7" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Karina</t>
+        </is>
+      </c>
+      <c r="B8" s="36" t="n">
+        <v>0.00663716814159292</v>
+      </c>
+      <c r="C8" s="53" t="n">
+        <v>0.254424778761062</v>
+      </c>
+      <c r="D8" s="42" t="n">
+        <v>0.1935840707964602</v>
+      </c>
+      <c r="E8" s="58" t="n">
+        <v>0.1360619469026549</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="49" t="n">
+        <v>0.1880530973451327</v>
+      </c>
+      <c r="H8" s="43" t="n">
+        <v>0.01769911504424779</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0.09845132743362832</v>
+      </c>
+      <c r="J8" s="24" t="n">
+        <v>0.1050884955752212</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Luisa</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Ricarda</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="75" t="n">
+        <v>0.002212389380530973</v>
+      </c>
+      <c r="D10" s="64" t="n">
+        <v>0.00995575221238938</v>
+      </c>
+      <c r="E10" s="47" t="n">
+        <v>0.02654867256637168</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="64" t="n">
+        <v>0.01106194690265487</v>
+      </c>
+      <c r="H10" s="82" t="n">
+        <v>0.9203539823008849</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="18" t="n">
+        <v>0.02986725663716814</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="B11" s="54" t="n">
+        <v>0.02323008849557522</v>
+      </c>
+      <c r="C11" s="41" t="n">
+        <v>0.08960176991150443</v>
+      </c>
+      <c r="D11" s="41" t="n">
+        <v>0.08849557522123894</v>
+      </c>
+      <c r="E11" s="83" t="n">
+        <v>0.2975663716814159</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="43" t="n">
+        <v>0.01769911504424779</v>
+      </c>
+      <c r="I11" s="53" t="n">
+        <v>0.2566371681415929</v>
+      </c>
+      <c r="J11" s="4" t="n">
+        <v>0.1106194690265487</v>
+      </c>
+      <c r="K11" s="27" t="n">
+        <v>0.1161504424778761</v>
+      </c>
+      <c r="L11" s="13" t="n">
+        <v>0.1084070796460177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added AYTO VIP S2 Episode 13 results
</commit_message>
<xml_diff>
--- a/results/AYTO VIP S2/results.xlsx
+++ b/results/AYTO VIP S2/results.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Episode 10" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Episode 11" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Episode 12" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Episode 13" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -45,7 +46,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="84">
+  <fills count="95">
     <fill>
       <patternFill/>
     </fill>
@@ -460,6 +461,61 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0021DEFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D12EFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004EB1FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000AF5FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0049B6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0024DBFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0044BBFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002ED1FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EA15FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003BC4FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005CA3FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0038C7FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -481,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -568,6 +624,17 @@
     <xf numFmtId="0" fontId="2" fillId="78" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="79" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="77" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="86" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="88" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="93" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="84" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="85" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="94" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="89" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="90" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="91" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="87" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="92" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -2355,6 +2422,482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amadu</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Luca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lukas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maurice</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pharrell</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B2" s="56" t="n">
+        <v>0.03403141361256545</v>
+      </c>
+      <c r="C2" s="17" t="n">
+        <v>0.06151832460732985</v>
+      </c>
+      <c r="D2" s="24" t="n">
+        <v>0.1020942408376963</v>
+      </c>
+      <c r="E2" s="84" t="n">
+        <v>0.0418848167539267</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="85" t="n">
+        <v>0.143979057591623</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11" t="n">
+        <v>0.06282722513089005</v>
+      </c>
+      <c r="J2" s="86" t="n">
+        <v>0.3599476439790576</v>
+      </c>
+      <c r="K2" s="42" t="n">
+        <v>0.193717277486911</v>
+      </c>
+      <c r="L2" s="13" t="n">
+        <v>0.1086387434554974</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cecilia</t>
+        </is>
+      </c>
+      <c r="B3" s="87" t="n">
+        <v>0.8167539267015707</v>
+      </c>
+      <c r="C3" s="74" t="n">
+        <v>0.0143979057591623</v>
+      </c>
+      <c r="D3" s="43" t="n">
+        <v>0.01701570680628272</v>
+      </c>
+      <c r="E3" s="74" t="n">
+        <v>0.01178010471204189</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="18" t="n">
+        <v>0.0274869109947644</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="34" t="n">
+        <v>0.04319371727748691</v>
+      </c>
+      <c r="J3" s="74" t="n">
+        <v>0.0143979057591623</v>
+      </c>
+      <c r="K3" s="15" t="n">
+        <v>0.0549738219895288</v>
+      </c>
+      <c r="L3" s="13" t="n">
+        <v>0.1086387434554974</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Celina</t>
+        </is>
+      </c>
+      <c r="B4" s="74" t="n">
+        <v>0.01308900523560209</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>0.08507853403141362</v>
+      </c>
+      <c r="D4" s="88" t="n">
+        <v>0.306282722513089</v>
+      </c>
+      <c r="E4" s="41" t="n">
+        <v>0.08638743455497382</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="22" t="n">
+        <v>0.1727748691099476</v>
+      </c>
+      <c r="H4" s="75" t="n">
+        <v>0.002617801047120419</v>
+      </c>
+      <c r="I4" s="41" t="n">
+        <v>0.08900523560209424</v>
+      </c>
+      <c r="J4" s="38" t="n">
+        <v>0.09554973821989529</v>
+      </c>
+      <c r="K4" s="61" t="n">
+        <v>0.1492146596858639</v>
+      </c>
+      <c r="L4" s="13" t="n">
+        <v>0.1086387434554974</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Franziska</t>
+        </is>
+      </c>
+      <c r="B5" s="40" t="n">
+        <v>0.04842931937172775</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>0.112565445026178</v>
+      </c>
+      <c r="D5" s="24" t="n">
+        <v>0.1047120418848168</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0.112565445026178</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="27" t="n">
+        <v>0.1138743455497382</v>
+      </c>
+      <c r="H5" s="74" t="n">
+        <v>0.01308900523560209</v>
+      </c>
+      <c r="I5" s="45" t="n">
+        <v>0.2107329842931937</v>
+      </c>
+      <c r="J5" s="11" t="n">
+        <v>0.06413612565445026</v>
+      </c>
+      <c r="K5" s="89" t="n">
+        <v>0.2198952879581152</v>
+      </c>
+      <c r="L5" s="13" t="n">
+        <v>0.1086387434554974</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+      <c r="B6" s="36" t="n">
+        <v>0.005235602094240838</v>
+      </c>
+      <c r="C6" s="60" t="n">
+        <v>0.2356020942408377</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0.08507853403141362</v>
+      </c>
+      <c r="E6" s="38" t="n">
+        <v>0.09554973821989529</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="46" t="n">
+        <v>0.09031413612565445</v>
+      </c>
+      <c r="H6" s="74" t="n">
+        <v>0.0143979057591623</v>
+      </c>
+      <c r="I6" s="61" t="n">
+        <v>0.1505235602094241</v>
+      </c>
+      <c r="J6" s="27" t="n">
+        <v>0.1138743455497382</v>
+      </c>
+      <c r="K6" s="45" t="n">
+        <v>0.2094240837696335</v>
+      </c>
+      <c r="L6" s="79" t="n">
+        <v>0.1308900523560209</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="B7" s="16" t="n">
+        <v>0.05104712041884817</v>
+      </c>
+      <c r="C7" s="58" t="n">
+        <v>0.1348167539267016</v>
+      </c>
+      <c r="D7" s="46" t="n">
+        <v>0.09162303664921466</v>
+      </c>
+      <c r="E7" s="66" t="n">
+        <v>0.1989528795811518</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="90" t="n">
+        <v>0.2683246073298429</v>
+      </c>
+      <c r="H7" s="54" t="n">
+        <v>0.02094240837696335</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>0.1099476439790576</v>
+      </c>
+      <c r="J7" s="62" t="n">
+        <v>0.1243455497382199</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="13" t="n">
+        <v>0.1086387434554974</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Karina</t>
+        </is>
+      </c>
+      <c r="B8" s="36" t="n">
+        <v>0.006544502617801047</v>
+      </c>
+      <c r="C8" s="21" t="n">
+        <v>0.2709424083769634</v>
+      </c>
+      <c r="D8" s="42" t="n">
+        <v>0.1924083769633508</v>
+      </c>
+      <c r="E8" s="58" t="n">
+        <v>0.1348167539267016</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="91" t="n">
+        <v>0.1806282722513089</v>
+      </c>
+      <c r="H8" s="64" t="n">
+        <v>0.01047120418848168</v>
+      </c>
+      <c r="I8" s="24" t="n">
+        <v>0.1020942408376963</v>
+      </c>
+      <c r="J8" s="24" t="n">
+        <v>0.1020942408376963</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="13" t="n">
+        <v>0.1086387434554974</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Luisa</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13" t="n">
+        <v>0.1086387434554974</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Ricarda</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="75" t="n">
+        <v>0.002617801047120419</v>
+      </c>
+      <c r="D10" s="64" t="n">
+        <v>0.01047120418848168</v>
+      </c>
+      <c r="E10" s="56" t="n">
+        <v>0.03141361256544502</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="75" t="n">
+        <v>0.002617801047120419</v>
+      </c>
+      <c r="H10" s="92" t="n">
+        <v>0.9175392670157068</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="71" t="n">
+        <v>0.03534031413612566</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="B11" s="47" t="n">
+        <v>0.02486910994764398</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>0.0824607329842932</v>
+      </c>
+      <c r="D11" s="46" t="n">
+        <v>0.09031413612565445</v>
+      </c>
+      <c r="E11" s="93" t="n">
+        <v>0.2866492146596858</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="54" t="n">
+        <v>0.02094240837696335</v>
+      </c>
+      <c r="I11" s="94" t="n">
+        <v>0.2316753926701571</v>
+      </c>
+      <c r="J11" s="33" t="n">
+        <v>0.1256544502617801</v>
+      </c>
+      <c r="K11" s="52" t="n">
+        <v>0.137434554973822</v>
+      </c>
+      <c r="L11" s="13" t="n">
+        <v>0.1086387434554974</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added AYTO VIP S2 Episode 14 results
</commit_message>
<xml_diff>
--- a/results/AYTO VIP S2/results.xlsx
+++ b/results/AYTO VIP S2/results.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Episode 11" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Episode 12" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Episode 13" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Episode 14" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -46,7 +47,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="95">
+  <fills count="103">
     <fill>
       <patternFill/>
     </fill>
@@ -516,6 +517,46 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0038C7FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BD42FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008877FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0034CBFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0042BDFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F00FFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007689FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002AD5FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0033CCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -537,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -635,6 +676,14 @@
     <xf numFmtId="0" fontId="3" fillId="91" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="87" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="92" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="100" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="95" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="96" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="101" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="97" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="98" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="99" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="102" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -2898,6 +2947,482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amadu</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Luca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lukas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maurice</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pharrell</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B2" s="84" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="C2" s="16" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="D2" s="76" t="n">
+        <v>0.1846153846153846</v>
+      </c>
+      <c r="E2" s="34" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.1128205128205128</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="15" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="J2" s="95" t="n">
+        <v>0.4615384615384616</v>
+      </c>
+      <c r="K2" s="34" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="L2" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cecilia</t>
+        </is>
+      </c>
+      <c r="B3" s="96" t="n">
+        <v>0.7384615384615385</v>
+      </c>
+      <c r="C3" s="36" t="n">
+        <v>0.005128205128205128</v>
+      </c>
+      <c r="D3" s="64" t="n">
+        <v>0.01025641025641026</v>
+      </c>
+      <c r="E3" s="84" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>0.08205128205128205</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="62" t="n">
+        <v>0.1230769230769231</v>
+      </c>
+      <c r="L3" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Celina</t>
+        </is>
+      </c>
+      <c r="B4" s="36" t="n">
+        <v>0.005128205128205128</v>
+      </c>
+      <c r="C4" s="14" t="n">
+        <v>0.1179487179487179</v>
+      </c>
+      <c r="D4" s="97" t="n">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="E4" s="74" t="n">
+        <v>0.01538461538461539</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>0.08205128205128205</v>
+      </c>
+      <c r="H4" s="36" t="n">
+        <v>0.005128205128205128</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>0.08205128205128205</v>
+      </c>
+      <c r="J4" s="74" t="n">
+        <v>0.01538461538461539</v>
+      </c>
+      <c r="K4" s="85" t="n">
+        <v>0.1435897435897436</v>
+      </c>
+      <c r="L4" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Franziska</t>
+        </is>
+      </c>
+      <c r="B5" s="33" t="n">
+        <v>0.1282051282051282</v>
+      </c>
+      <c r="C5" s="46" t="n">
+        <v>0.09230769230769231</v>
+      </c>
+      <c r="D5" s="17" t="n">
+        <v>0.06153846153846154</v>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="49" t="n">
+        <v>0.1897435897435897</v>
+      </c>
+      <c r="H5" s="64" t="n">
+        <v>0.01025641025641026</v>
+      </c>
+      <c r="I5" s="33" t="n">
+        <v>0.1282051282051282</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="37" t="n">
+        <v>0.3230769230769231</v>
+      </c>
+      <c r="L5" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="57" t="n">
+        <v>0.3641025641025641</v>
+      </c>
+      <c r="D6" s="54" t="n">
+        <v>0.02051282051282051</v>
+      </c>
+      <c r="E6" s="17" t="n">
+        <v>0.06153846153846154</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="80" t="n">
+        <v>0.1692307692307692</v>
+      </c>
+      <c r="H6" s="36" t="n">
+        <v>0.005128205128205128</v>
+      </c>
+      <c r="I6" s="34" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="J6" s="80" t="n">
+        <v>0.1692307692307692</v>
+      </c>
+      <c r="K6" s="98" t="n">
+        <v>0.1641025641025641</v>
+      </c>
+      <c r="L6" s="78" t="n">
+        <v>0.1794871794871795</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="B7" s="84" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="C7" s="13" t="n">
+        <v>0.1076923076923077</v>
+      </c>
+      <c r="D7" s="54" t="n">
+        <v>0.02051282051282051</v>
+      </c>
+      <c r="E7" s="99" t="n">
+        <v>0.2051282051282051</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="100" t="n">
+        <v>0.2615384615384616</v>
+      </c>
+      <c r="H7" s="84" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="I7" s="80" t="n">
+        <v>0.1692307692307692</v>
+      </c>
+      <c r="J7" s="63" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Karina</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="61" t="n">
+        <v>0.1487179487179487</v>
+      </c>
+      <c r="D8" s="10" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="E8" s="31" t="n">
+        <v>0.2769230769230769</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="22" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25" t="n">
+        <v>0.282051282051282</v>
+      </c>
+      <c r="J8" s="16" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Luisa</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Ricarda</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="64" t="n">
+        <v>0.01025641025641026</v>
+      </c>
+      <c r="D10" s="84" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="64" t="n">
+        <v>0.01025641025641026</v>
+      </c>
+      <c r="H10" s="101" t="n">
+        <v>0.9384615384615385</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="B11" s="34" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="C11" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+      <c r="D11" s="17" t="n">
+        <v>0.06153846153846154</v>
+      </c>
+      <c r="E11" s="93" t="n">
+        <v>0.2871794871794872</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="63" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="J11" s="61" t="n">
+        <v>0.1487179487179487</v>
+      </c>
+      <c r="K11" s="102" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L11" s="24" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added AYTO VIP S2 Episode 15 results
</commit_message>
<xml_diff>
--- a/results/AYTO VIP S2/results.xlsx
+++ b/results/AYTO VIP S2/results.xlsx
@@ -20,6 +20,7 @@
     <sheet name="Episode 12" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Episode 13" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Episode 14" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Episode 15" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -47,7 +48,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="103">
+  <fills count="109">
     <fill>
       <patternFill/>
     </fill>
@@ -557,6 +558,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0033CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00639CFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00609FFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005AA5FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00718EFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0051AEFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0037C8FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -578,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -684,6 +715,12 @@
     <xf numFmtId="0" fontId="2" fillId="98" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="99" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="102" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="106" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="103" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="107" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="105" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="104" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="108" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -3423,6 +3460,482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amadu</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Luca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lukas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maurice</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pharrell</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>0.06944444444444445</v>
+      </c>
+      <c r="D2" s="51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="11" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="84" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0.0763888888888889</v>
+      </c>
+      <c r="J2" s="103" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="K2" s="15" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="L2" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cecilia</t>
+        </is>
+      </c>
+      <c r="B3" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Celina</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="70" t="n">
+        <v>0.1597222222222222</v>
+      </c>
+      <c r="D4" s="104" t="n">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E4" s="54" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24" t="n">
+        <v>0.1041666666666667</v>
+      </c>
+      <c r="H4" s="36" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J4" s="54" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="K4" s="49" t="n">
+        <v>0.1875</v>
+      </c>
+      <c r="L4" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Franziska</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="E5" s="46" t="n">
+        <v>0.09027777777777778</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="53" t="n">
+        <v>0.2569444444444444</v>
+      </c>
+      <c r="H5" s="74" t="n">
+        <v>0.01388888888888889</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="105" t="n">
+        <v>0.3194444444444444</v>
+      </c>
+      <c r="L5" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="48" t="n">
+        <v>0.1458333333333333</v>
+      </c>
+      <c r="D6" s="18" t="n">
+        <v>0.02777777777777778</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="81" t="n">
+        <v>0.2291666666666667</v>
+      </c>
+      <c r="H6" s="36" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="J6" s="89" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="K6" s="89" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="L6" s="89" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="48" t="n">
+        <v>0.1458333333333333</v>
+      </c>
+      <c r="D7" s="18" t="n">
+        <v>0.02777777777777778</v>
+      </c>
+      <c r="E7" s="46" t="n">
+        <v>0.09027777777777778</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="106" t="n">
+        <v>0.3541666666666667</v>
+      </c>
+      <c r="H7" s="15" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="I7" s="22" t="n">
+        <v>0.1736111111111111</v>
+      </c>
+      <c r="J7" s="63" t="n">
+        <v>0.1527777777777778</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Karina</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="102" t="n">
+        <v>0.2013888888888889</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="E8" s="107" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="J8" s="74" t="n">
+        <v>0.01388888888888889</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Luisa</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Ricarda</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="74" t="n">
+        <v>0.01388888888888889</v>
+      </c>
+      <c r="D10" s="15" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="74" t="n">
+        <v>0.01388888888888889</v>
+      </c>
+      <c r="H10" s="92" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="52" t="n">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="E11" s="26" t="n">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="52" t="n">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="J11" s="48" t="n">
+        <v>0.1458333333333333</v>
+      </c>
+      <c r="K11" s="108" t="n">
+        <v>0.2152777777777778</v>
+      </c>
+      <c r="L11" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added AYTO VIP S2 Episode 16 results
</commit_message>
<xml_diff>
--- a/results/AYTO VIP S2/results.xlsx
+++ b/results/AYTO VIP S2/results.xlsx
@@ -21,6 +21,7 @@
     <sheet name="Episode 13" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Episode 14" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Episode 15" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Episode 16" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3936,6 +3937,482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amadu</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Luca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lukas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maurice</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pharrell</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>0.06944444444444445</v>
+      </c>
+      <c r="D2" s="51" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="11" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="84" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0.0763888888888889</v>
+      </c>
+      <c r="J2" s="103" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="K2" s="15" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="L2" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cecilia</t>
+        </is>
+      </c>
+      <c r="B3" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Celina</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="70" t="n">
+        <v>0.1597222222222222</v>
+      </c>
+      <c r="D4" s="104" t="n">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E4" s="54" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24" t="n">
+        <v>0.1041666666666667</v>
+      </c>
+      <c r="H4" s="36" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J4" s="54" t="n">
+        <v>0.02083333333333333</v>
+      </c>
+      <c r="K4" s="49" t="n">
+        <v>0.1875</v>
+      </c>
+      <c r="L4" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Franziska</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="E5" s="46" t="n">
+        <v>0.09027777777777778</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="53" t="n">
+        <v>0.2569444444444444</v>
+      </c>
+      <c r="H5" s="74" t="n">
+        <v>0.01388888888888889</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="105" t="n">
+        <v>0.3194444444444444</v>
+      </c>
+      <c r="L5" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="48" t="n">
+        <v>0.1458333333333333</v>
+      </c>
+      <c r="D6" s="18" t="n">
+        <v>0.02777777777777778</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="81" t="n">
+        <v>0.2291666666666667</v>
+      </c>
+      <c r="H6" s="36" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="J6" s="89" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="K6" s="89" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="L6" s="89" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="48" t="n">
+        <v>0.1458333333333333</v>
+      </c>
+      <c r="D7" s="18" t="n">
+        <v>0.02777777777777778</v>
+      </c>
+      <c r="E7" s="46" t="n">
+        <v>0.09027777777777778</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="106" t="n">
+        <v>0.3541666666666667</v>
+      </c>
+      <c r="H7" s="15" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="I7" s="22" t="n">
+        <v>0.1736111111111111</v>
+      </c>
+      <c r="J7" s="63" t="n">
+        <v>0.1527777777777778</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Karina</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="102" t="n">
+        <v>0.2013888888888889</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="E8" s="107" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="J8" s="74" t="n">
+        <v>0.01388888888888889</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Luisa</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Ricarda</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="74" t="n">
+        <v>0.01388888888888889</v>
+      </c>
+      <c r="D10" s="15" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="74" t="n">
+        <v>0.01388888888888889</v>
+      </c>
+      <c r="H10" s="92" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="52" t="n">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="E11" s="26" t="n">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="52" t="n">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="J11" s="48" t="n">
+        <v>0.1458333333333333</v>
+      </c>
+      <c r="K11" s="108" t="n">
+        <v>0.2152777777777778</v>
+      </c>
+      <c r="L11" s="38" t="n">
+        <v>0.09722222222222222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added AYTO VIP S2 Episode 17 results
</commit_message>
<xml_diff>
--- a/results/AYTO VIP S2/results.xlsx
+++ b/results/AYTO VIP S2/results.xlsx
@@ -22,6 +22,7 @@
     <sheet name="Episode 14" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Episode 15" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Episode 16" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Episode 17" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -49,7 +50,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="109">
+  <fills count="114">
     <fill>
       <patternFill/>
     </fill>
@@ -589,6 +590,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0037C8FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A05FFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00946BFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00748BFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D02FFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006897FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -610,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -722,6 +748,11 @@
     <xf numFmtId="0" fontId="3" fillId="105" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="104" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="108" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="109" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="111" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="110" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="112" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="113" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -4413,6 +4444,482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amadu</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Luca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lukas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maurice</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pharrell</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cecilia</t>
+        </is>
+      </c>
+      <c r="B3" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Celina</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+      <c r="D4" s="109" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="70" t="n">
+        <v>0.15625</v>
+      </c>
+      <c r="H4" s="43" t="n">
+        <v>0.015625</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>0.109375</v>
+      </c>
+      <c r="L4" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Franziska</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="70" t="n">
+        <v>0.15625</v>
+      </c>
+      <c r="D5" s="40" t="n">
+        <v>0.046875</v>
+      </c>
+      <c r="E5" s="33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="110" t="n">
+        <v>0.453125</v>
+      </c>
+      <c r="H5" s="56" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="49" t="n">
+        <v>0.1875</v>
+      </c>
+      <c r="L5" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="56" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="D6" s="40" t="n">
+        <v>0.046875</v>
+      </c>
+      <c r="E6" s="33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="86" t="n">
+        <v>0.359375</v>
+      </c>
+      <c r="H6" s="43" t="n">
+        <v>0.015625</v>
+      </c>
+      <c r="I6" s="33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="83" t="n">
+        <v>0.296875</v>
+      </c>
+      <c r="L6" s="51" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="25" t="n">
+        <v>0.28125</v>
+      </c>
+      <c r="D7" s="40" t="n">
+        <v>0.046875</v>
+      </c>
+      <c r="E7" s="22" t="n">
+        <v>0.171875</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="I7" s="107" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Karina</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="E8" s="111" t="n">
+        <v>0.578125</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="60" t="n">
+        <v>0.234375</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Luisa</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Ricarda</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="56" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="D10" s="33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="56" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="H10" s="112" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="25" t="n">
+        <v>0.28125</v>
+      </c>
+      <c r="D11" s="40" t="n">
+        <v>0.046875</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="90" t="n">
+        <v>0.265625</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="113" t="n">
+        <v>0.40625</v>
+      </c>
+      <c r="L11" s="38" t="n">
+        <v>0.09375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added AYTO VIP S2 Episode 18 results
</commit_message>
<xml_diff>
--- a/results/AYTO VIP S2/results.xlsx
+++ b/results/AYTO VIP S2/results.xlsx
@@ -23,6 +23,7 @@
     <sheet name="Episode 15" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Episode 16" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="Episode 17" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Episode 18" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4920,6 +4921,482 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amadu</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Calvin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fabio</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Luca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lukas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Maurice</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pharrell</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Felix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cecilia</t>
+        </is>
+      </c>
+      <c r="B3" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Celina</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Franziska</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gina</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Karina</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Luisa</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Ricarda</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>